<commit_message>
Travail sur les imports
</commit_message>
<xml_diff>
--- a/updates/excels/contacts.xlsx
+++ b/updates/excels/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\wakaari\plugins\waka\crsm\updates\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF21A51-A2A9-474B-A342-2F17075DD352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4ED072-4A5A-410B-9DE8-F32B9B3F4237}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{9D1F2406-6DE7-4E0A-8ABE-1B0E9B1385AD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -48,13 +48,28 @@
     <t>client</t>
   </si>
   <si>
-    <t>glllllllevents</t>
-  </si>
-  <si>
-    <t>glllleeeeevvents</t>
-  </si>
-  <si>
     <t>evolutic</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>EEE</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>FFF</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>jaqussd</t>
+  </si>
+  <si>
+    <t>vvvvv</t>
   </si>
 </sst>
 </file>
@@ -406,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B6C717-B60A-418B-A0B8-D43F70DEF730}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -431,24 +446,51 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>